<commit_message>
add back generated data without conflict rate add bash script to run for all conflict rates add script to evaluate solver run times update README.md update graph line design
</commit_message>
<xml_diff>
--- a/results/conf_progression.xlsx
+++ b/results/conf_progression.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34125" windowHeight="17835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,6 +255,7 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -357,11 +358,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1392049664"/>
-        <c:axId val="-1392039328"/>
+        <c:axId val="-1759322752"/>
+        <c:axId val="-1759323296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1392049664"/>
+        <c:axId val="-1759322752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +453,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1392039328"/>
+        <c:crossAx val="-1759323296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -460,7 +461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1392039328"/>
+        <c:axId val="-1759323296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -560,7 +561,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1392049664"/>
+        <c:crossAx val="-1759322752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1411,7 +1412,7 @@
       <sheetName val="2016-11-07-4"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="89">
           <cell r="D89">
@@ -1424,30 +1425,30 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2311,7 +2312,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update conf results with workload performance indicators
</commit_message>
<xml_diff>
--- a/results/conf_progression.xlsx
+++ b/results/conf_progression.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groschri\Seafile\My Library\uni\long-term-fairness\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groschri\Seafile\My Library\uni\long-term-workload\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,12 +37,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>APS</t>
   </si>
   <si>
-    <t>APV</t>
+    <t>ASV</t>
+  </si>
+  <si>
+    <t>APL</t>
+  </si>
+  <si>
+    <t>ALV</t>
+  </si>
+  <si>
+    <t>conf. rate</t>
   </si>
 </sst>
 </file>
@@ -202,34 +211,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.224813186635114E-2</c:v>
+                  <c:v>-2.7971027175238614E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.2608652036338539</c:v>
+                  <c:v>5.3382817938382983E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.42117416749225373</c:v>
+                  <c:v>1.6230886980694286E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.66636390050646099</c:v>
+                  <c:v>-6.3418440785472374E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.67958437524874538</c:v>
+                  <c:v>-1.4540055900507096E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.76693053914773313</c:v>
+                  <c:v>-4.1596161053225299E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.90003198143220642</c:v>
+                  <c:v>-5.9482533029348784E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.94403406283333358</c:v>
+                  <c:v>-0.14115539924792178</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.96496810778391373</c:v>
+                  <c:v>-0.15566662571041948</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.99641276837750237</c:v>
+                  <c:v>-7.7783515544197671E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -245,7 +254,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>APV</c:v>
+                  <c:v>ASV</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -315,34 +324,260 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.6799354798089723E-2</c:v>
+                  <c:v>-3.7178053505118186E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.1310855075380663</c:v>
+                  <c:v>-7.9639926728015328E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.19854805008087886</c:v>
+                  <c:v>-1.3086940552413839E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.2364802448653196</c:v>
+                  <c:v>-2.2227778622953397E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.29684368483689794</c:v>
+                  <c:v>-5.8178070445915601E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.3675586126986351</c:v>
+                  <c:v>-7.8348751953718293E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.40466640802909237</c:v>
+                  <c:v>-9.3603952065196283E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.399393286991156</c:v>
+                  <c:v>-0.11038859617038539</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.42878842634149705</c:v>
+                  <c:v>-0.13492473240673331</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.77475110588747431</c:v>
+                  <c:v>-0.11726771819964622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>APL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-0.12323057161976494</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.23164089300678684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.30233649734013579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.32328567629518573</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.21298388953801081</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.10802485383342604</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.1449782781520764</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.26905048251079527</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.17084212574267765</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.16615310187323939</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.39300916062583441</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ALV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-9.181563099207686E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.11149714837440589</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.12457175817247712</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.11515051463516163</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.12231013154534005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.15100636878708529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.15075297494221235</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.16985860672015232</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.15006777064057977</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.14708943076262754</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.24416150652844293</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,11 +593,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1759322752"/>
-        <c:axId val="-1759323296"/>
+        <c:axId val="173086432"/>
+        <c:axId val="173085344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1759322752"/>
+        <c:axId val="173086432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +660,7 @@
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="high"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -453,7 +688,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1759323296"/>
+        <c:crossAx val="173085344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -461,7 +696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1759323296"/>
+        <c:axId val="173085344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -561,7 +796,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1759322752"/>
+        <c:crossAx val="173086432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1201,16 +1436,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>580350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>63412</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>177712</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1238,42 +1473,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
+      <sheetName val="2016-01-04-4"/>
+      <sheetName val="2017-10-02-5"/>
+      <sheetName val="2016-12-05-5"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2017-02-06-4"/>
+      <sheetName val="2017-08-07-4"/>
+      <sheetName val="2017-09-04-4"/>
+      <sheetName val="2016-08-01-5"/>
       <sheetName val="2016-09-05-4"/>
+      <sheetName val="2017-07-03-5"/>
       <sheetName val="2016-10-03-5"/>
       <sheetName val="2015-12-07-4"/>
-      <sheetName val="2017-09-04-4"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2016-01-04-4"/>
-      <sheetName val="2017-01-09-4"/>
-      <sheetName val="2017-05-01-5"/>
-      <sheetName val="2016-08-01-5"/>
-      <sheetName val="2017-08-07-4"/>
+      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2016-05-02-5"/>
       <sheetName val="2016-04-04-4"/>
+      <sheetName val="2016-06-06-4"/>
       <sheetName val="2016-03-07-4"/>
+      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2016-02-01-5"/>
       <sheetName val="2016-07-04-4"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2017-07-03-5"/>
-      <sheetName val="2016-11-07-4"/>
       <sheetName val="2017-04-03-4"/>
-      <sheetName val="2016-05-02-5"/>
-      <sheetName val="2016-12-05-5"/>
-      <sheetName val="2017-03-06-4"/>
-      <sheetName val="2017-02-06-4"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2016-06-06-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
+          <cell r="I89">
             <v>0</v>
+          </cell>
+          <cell r="M89">
+            <v>-9.1815630992076862</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
+          <cell r="H92">
             <v>0</v>
+          </cell>
+          <cell r="L92">
+            <v>-12.323057161976495</v>
           </cell>
         </row>
       </sheetData>
@@ -1312,42 +1553,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
-      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2016-08-01-5"/>
+      <sheetName val="2017-07-03-5"/>
+      <sheetName val="2017-10-02-5"/>
+      <sheetName val="2016-01-04-4"/>
+      <sheetName val="2016-09-05-4"/>
       <sheetName val="2016-07-04-4"/>
-      <sheetName val="2017-09-04-4"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2016-04-04-4"/>
       <sheetName val="2016-03-07-4"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2016-08-01-5"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2017-02-06-4"/>
-      <sheetName val="2017-08-07-4"/>
-      <sheetName val="2016-12-05-5"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2016-10-03-5"/>
-      <sheetName val="2016-01-04-4"/>
-      <sheetName val="2017-01-09-4"/>
-      <sheetName val="2016-04-04-4"/>
-      <sheetName val="2017-04-03-4"/>
-      <sheetName val="2017-07-03-5"/>
-      <sheetName val="2016-06-06-4"/>
-      <sheetName val="2017-05-01-5"/>
       <sheetName val="2016-05-02-5"/>
       <sheetName val="2016-11-07-4"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2017-08-07-4"/>
+      <sheetName val="2016-06-06-4"/>
+      <sheetName val="2016-12-05-5"/>
+      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2017-09-04-4"/>
+      <sheetName val="2017-02-06-4"/>
+      <sheetName val="2016-02-01-5"/>
       <sheetName val="2015-12-07-4"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2016-10-03-5"/>
+      <sheetName val="2017-04-03-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-42.878842634149706</v>
+          <cell r="I89">
+            <v>-13.492473240673331</v>
+          </cell>
+          <cell r="M89">
+            <v>-14.708943076262754</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-96.496810778391378</v>
+          <cell r="H92">
+            <v>-15.566662571041947</v>
+          </cell>
+          <cell r="L92">
+            <v>-16.615310187323939</v>
           </cell>
         </row>
       </sheetData>
@@ -1386,69 +1633,75 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
+      <sheetName val="2016-04-04-4"/>
+      <sheetName val="2016-12-05-5"/>
+      <sheetName val="2015-12-07-4"/>
       <sheetName val="2015-11-02-5"/>
+      <sheetName val="2016-09-05-4"/>
+      <sheetName val="2016-01-04-4"/>
+      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2016-06-06-4"/>
+      <sheetName val="2017-02-06-4"/>
+      <sheetName val="2016-08-01-5"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2017-07-03-5"/>
+      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2017-04-03-4"/>
+      <sheetName val="2016-10-03-5"/>
       <sheetName val="2017-08-07-4"/>
+      <sheetName val="2016-07-04-4"/>
+      <sheetName val="2016-05-02-5"/>
+      <sheetName val="2016-03-07-4"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2017-10-02-5"/>
       <sheetName val="2017-01-09-4"/>
-      <sheetName val="2016-01-04-4"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2017-07-03-5"/>
+      <sheetName val="2016-02-01-5"/>
       <sheetName val="2017-09-04-4"/>
-      <sheetName val="2016-07-04-4"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2017-03-06-4"/>
-      <sheetName val="2016-04-04-4"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2015-12-07-4"/>
-      <sheetName val="2016-06-06-4"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2016-03-07-4"/>
-      <sheetName val="2016-08-01-5"/>
-      <sheetName val="2017-04-03-4"/>
-      <sheetName val="2017-05-01-5"/>
-      <sheetName val="2016-12-05-5"/>
-      <sheetName val="2016-10-03-5"/>
-      <sheetName val="2017-02-06-4"/>
-      <sheetName val="2016-05-02-5"/>
-      <sheetName val="2016-11-07-4"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-77.475110588747427</v>
+          <cell r="I89">
+            <v>-11.726771819964622</v>
+          </cell>
+          <cell r="M89">
+            <v>-24.416150652844294</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-99.64127683775024</v>
+          <cell r="H92">
+            <v>-7.7783515544197668</v>
+          </cell>
+          <cell r="L92">
+            <v>-39.30091606258344</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1460,42 +1713,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
+      <sheetName val="2016-09-05-4"/>
+      <sheetName val="2017-09-04-4"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2016-10-03-5"/>
+      <sheetName val="2016-06-06-4"/>
+      <sheetName val="2017-02-06-4"/>
+      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2016-07-04-4"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2016-12-05-5"/>
+      <sheetName val="2017-10-02-5"/>
+      <sheetName val="2017-07-03-5"/>
+      <sheetName val="2016-02-01-5"/>
+      <sheetName val="2016-04-04-4"/>
+      <sheetName val="2016-05-02-5"/>
       <sheetName val="2017-08-07-4"/>
-      <sheetName val="2017-03-06-4"/>
-      <sheetName val="2016-06-06-4"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2017-02-06-4"/>
       <sheetName val="2016-08-01-5"/>
+      <sheetName val="2016-03-07-4"/>
+      <sheetName val="2016-01-04-4"/>
       <sheetName val="2016-11-07-4"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2016-12-05-5"/>
-      <sheetName val="2016-03-07-4"/>
-      <sheetName val="2017-01-09-4"/>
-      <sheetName val="2016-01-04-4"/>
-      <sheetName val="2016-07-04-4"/>
-      <sheetName val="2017-07-03-5"/>
-      <sheetName val="2016-05-02-5"/>
+      <sheetName val="2015-11-02-5"/>
       <sheetName val="2015-12-07-4"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2016-10-03-5"/>
-      <sheetName val="2017-09-04-4"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2016-04-04-4"/>
       <sheetName val="2017-04-03-4"/>
-      <sheetName val="2017-05-01-5"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-5.6799354798089725</v>
+          <cell r="I89">
+            <v>-0.37178053505118186</v>
+          </cell>
+          <cell r="M89">
+            <v>-11.149714837440589</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-5.2248131866351137</v>
+          <cell r="H92">
+            <v>-2.7971027175238614</v>
+          </cell>
+          <cell r="L92">
+            <v>-23.164089300678683</v>
           </cell>
         </row>
       </sheetData>
@@ -1534,42 +1793,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
+      <sheetName val="2017-04-03-4"/>
+      <sheetName val="2016-09-05-4"/>
+      <sheetName val="2016-07-04-4"/>
+      <sheetName val="2016-10-03-5"/>
+      <sheetName val="2017-09-04-4"/>
+      <sheetName val="2017-06-05-4"/>
       <sheetName val="2016-04-04-4"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2017-09-04-4"/>
       <sheetName val="2017-03-06-4"/>
+      <sheetName val="2017-07-03-5"/>
       <sheetName val="2017-02-06-4"/>
+      <sheetName val="2017-08-07-4"/>
+      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2017-10-02-5"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2016-03-07-4"/>
+      <sheetName val="2016-01-04-4"/>
       <sheetName val="2016-05-02-5"/>
+      <sheetName val="2016-12-05-5"/>
       <sheetName val="2017-01-09-4"/>
+      <sheetName val="2015-12-07-4"/>
+      <sheetName val="2016-08-01-5"/>
+      <sheetName val="2016-02-01-5"/>
       <sheetName val="2016-06-06-4"/>
-      <sheetName val="2017-04-03-4"/>
-      <sheetName val="2016-03-07-4"/>
-      <sheetName val="2017-05-01-5"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2016-01-04-4"/>
-      <sheetName val="2016-07-04-4"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2016-08-01-5"/>
-      <sheetName val="2016-10-03-5"/>
-      <sheetName val="2016-12-05-5"/>
-      <sheetName val="2015-12-07-4"/>
-      <sheetName val="2016-11-07-4"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2017-07-03-5"/>
-      <sheetName val="2017-08-07-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-13.108550753806631</v>
+          <cell r="I89">
+            <v>-0.79639926728015331</v>
+          </cell>
+          <cell r="M89">
+            <v>-12.457175817247713</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-26.086520363385389</v>
+          <cell r="H92">
+            <v>0.53382817938382987</v>
+          </cell>
+          <cell r="L92">
+            <v>-30.233649734013579</v>
           </cell>
         </row>
       </sheetData>
@@ -1608,42 +1873,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
+      <sheetName val="2016-04-04-4"/>
       <sheetName val="2017-04-03-4"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2016-04-04-4"/>
-      <sheetName val="2015-12-07-4"/>
-      <sheetName val="2017-02-06-4"/>
-      <sheetName val="2017-07-03-5"/>
-      <sheetName val="2016-06-06-4"/>
-      <sheetName val="2016-05-02-5"/>
+      <sheetName val="2016-09-05-4"/>
+      <sheetName val="2016-03-07-4"/>
+      <sheetName val="2016-02-01-5"/>
       <sheetName val="2016-07-04-4"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2017-03-06-4"/>
       <sheetName val="2016-10-03-5"/>
       <sheetName val="2017-10-02-5"/>
+      <sheetName val="2017-09-04-4"/>
+      <sheetName val="2017-02-06-4"/>
+      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2016-06-06-4"/>
+      <sheetName val="2017-07-03-5"/>
+      <sheetName val="2016-12-05-5"/>
+      <sheetName val="2015-12-07-4"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2017-03-06-4"/>
       <sheetName val="2016-01-04-4"/>
-      <sheetName val="2017-09-04-4"/>
-      <sheetName val="2017-08-07-4"/>
-      <sheetName val="2016-03-07-4"/>
       <sheetName val="2016-11-07-4"/>
       <sheetName val="2016-08-01-5"/>
-      <sheetName val="2016-12-05-5"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2017-01-09-4"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2016-05-02-5"/>
+      <sheetName val="2017-08-07-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-19.854805008087887</v>
+          <cell r="I89">
+            <v>-1.3086940552413839</v>
+          </cell>
+          <cell r="M89">
+            <v>-11.515051463516162</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-42.11741674922537</v>
+          <cell r="H92">
+            <v>1.6230886980694286</v>
+          </cell>
+          <cell r="L92">
+            <v>-32.328567629518574</v>
           </cell>
         </row>
       </sheetData>
@@ -1682,42 +1953,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
+      <sheetName val="2015-12-07-4"/>
+      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2016-12-05-5"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2016-10-03-5"/>
+      <sheetName val="2017-07-03-5"/>
+      <sheetName val="2017-02-06-4"/>
+      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2016-07-04-4"/>
+      <sheetName val="2016-02-01-5"/>
+      <sheetName val="2017-08-07-4"/>
+      <sheetName val="2016-09-05-4"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2016-05-02-5"/>
+      <sheetName val="2017-04-03-4"/>
+      <sheetName val="2016-08-01-5"/>
+      <sheetName val="2017-09-04-4"/>
+      <sheetName val="2016-06-06-4"/>
+      <sheetName val="2016-04-04-4"/>
+      <sheetName val="2017-10-02-5"/>
+      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2016-01-04-4"/>
       <sheetName val="2016-03-07-4"/>
-      <sheetName val="2016-07-04-4"/>
-      <sheetName val="2016-01-04-4"/>
-      <sheetName val="2015-12-07-4"/>
-      <sheetName val="2016-11-07-4"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2016-06-06-4"/>
-      <sheetName val="2017-08-07-4"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2016-10-03-5"/>
-      <sheetName val="2017-09-04-4"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2017-07-03-5"/>
-      <sheetName val="2016-08-01-5"/>
-      <sheetName val="2016-05-02-5"/>
-      <sheetName val="2017-05-01-5"/>
-      <sheetName val="2017-04-03-4"/>
-      <sheetName val="2016-12-05-5"/>
-      <sheetName val="2017-02-06-4"/>
-      <sheetName val="2017-01-09-4"/>
-      <sheetName val="2017-03-06-4"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2016-04-04-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-23.648024486531959</v>
+          <cell r="I89">
+            <v>-2.2227778622953398</v>
+          </cell>
+          <cell r="M89">
+            <v>-12.231013154534006</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-66.636390050646099</v>
+          <cell r="H92">
+            <v>-6.3418440785472372</v>
+          </cell>
+          <cell r="L92">
+            <v>-21.29838895380108</v>
           </cell>
         </row>
       </sheetData>
@@ -1756,42 +2033,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
-      <sheetName val="2016-03-07-4"/>
-      <sheetName val="2016-01-04-4"/>
+      <sheetName val="2017-04-03-4"/>
+      <sheetName val="2016-10-03-5"/>
+      <sheetName val="2016-02-01-5"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2017-02-06-4"/>
+      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2016-07-04-4"/>
+      <sheetName val="2016-06-06-4"/>
+      <sheetName val="2017-01-09-4"/>
       <sheetName val="2017-07-03-5"/>
-      <sheetName val="2016-10-03-5"/>
-      <sheetName val="2016-04-04-4"/>
+      <sheetName val="2017-08-07-4"/>
       <sheetName val="2016-09-05-4"/>
       <sheetName val="2017-10-02-5"/>
       <sheetName val="2016-05-02-5"/>
-      <sheetName val="2017-01-09-4"/>
-      <sheetName val="2016-06-06-4"/>
-      <sheetName val="2017-08-07-4"/>
-      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2016-08-01-5"/>
       <sheetName val="2016-12-05-5"/>
-      <sheetName val="2016-07-04-4"/>
-      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2015-12-07-4"/>
       <sheetName val="2017-05-01-5"/>
+      <sheetName val="2016-03-07-4"/>
+      <sheetName val="2016-04-04-4"/>
+      <sheetName val="2016-01-04-4"/>
       <sheetName val="2017-09-04-4"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2015-12-07-4"/>
-      <sheetName val="2016-02-01-5"/>
       <sheetName val="2016-11-07-4"/>
-      <sheetName val="2017-02-06-4"/>
-      <sheetName val="2016-08-01-5"/>
-      <sheetName val="2017-04-03-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-29.684368483689795</v>
+          <cell r="I89">
+            <v>-5.81780704459156</v>
+          </cell>
+          <cell r="M89">
+            <v>-15.100636878708528</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-67.95843752487454</v>
+          <cell r="H92">
+            <v>-1.4540055900507096</v>
+          </cell>
+          <cell r="L92">
+            <v>-10.802485383342605</v>
           </cell>
         </row>
       </sheetData>
@@ -1830,42 +2113,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
+      <sheetName val="2016-09-05-4"/>
+      <sheetName val="2016-07-04-4"/>
+      <sheetName val="2017-07-03-5"/>
+      <sheetName val="2016-01-04-4"/>
+      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2016-03-07-4"/>
+      <sheetName val="2016-10-03-5"/>
+      <sheetName val="2015-12-07-4"/>
+      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2017-08-07-4"/>
+      <sheetName val="2016-05-02-5"/>
+      <sheetName val="2017-09-04-4"/>
+      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2017-04-03-4"/>
       <sheetName val="2016-08-01-5"/>
-      <sheetName val="2016-05-02-5"/>
-      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2017-10-02-5"/>
+      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2016-02-01-5"/>
+      <sheetName val="2016-12-05-5"/>
       <sheetName val="2017-02-06-4"/>
-      <sheetName val="2017-04-03-4"/>
-      <sheetName val="2017-08-07-4"/>
-      <sheetName val="2016-02-01-5"/>
+      <sheetName val="2017-05-01-5"/>
       <sheetName val="2016-04-04-4"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2017-09-04-4"/>
-      <sheetName val="2016-10-03-5"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2017-03-06-4"/>
-      <sheetName val="2016-12-05-5"/>
-      <sheetName val="2016-01-04-4"/>
-      <sheetName val="2015-12-07-4"/>
-      <sheetName val="2017-05-01-5"/>
-      <sheetName val="2016-03-07-4"/>
       <sheetName val="2016-06-06-4"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2017-07-03-5"/>
-      <sheetName val="2016-07-04-4"/>
-      <sheetName val="2017-01-09-4"/>
-      <sheetName val="2017-06-05-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-36.755861269863509</v>
+          <cell r="I89">
+            <v>-7.8348751953718292</v>
+          </cell>
+          <cell r="M89">
+            <v>-15.075297494221235</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-76.693053914773316</v>
+          <cell r="H92">
+            <v>-4.15961610532253</v>
+          </cell>
+          <cell r="L92">
+            <v>-14.497827815207639</v>
           </cell>
         </row>
       </sheetData>
@@ -1904,42 +2193,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
-      <sheetName val="2017-01-09-4"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2017-10-02-5"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2016-03-07-4"/>
+      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2016-07-04-4"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2015-12-07-4"/>
       <sheetName val="2016-06-06-4"/>
       <sheetName val="2016-12-05-5"/>
-      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2017-08-07-4"/>
+      <sheetName val="2015-11-02-5"/>
+      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2017-04-03-4"/>
+      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2016-05-02-5"/>
+      <sheetName val="2016-01-04-4"/>
+      <sheetName val="2017-09-04-4"/>
+      <sheetName val="2016-09-05-4"/>
+      <sheetName val="2016-04-04-4"/>
+      <sheetName val="2016-02-01-5"/>
+      <sheetName val="2016-08-01-5"/>
+      <sheetName val="2017-02-06-4"/>
       <sheetName val="2017-07-03-5"/>
-      <sheetName val="2017-08-07-4"/>
-      <sheetName val="2017-03-06-4"/>
-      <sheetName val="2016-07-04-4"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2016-04-04-4"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2017-02-06-4"/>
-      <sheetName val="2016-08-01-5"/>
-      <sheetName val="2016-03-07-4"/>
-      <sheetName val="2015-12-07-4"/>
-      <sheetName val="2017-04-03-4"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2017-09-04-4"/>
-      <sheetName val="2016-05-02-5"/>
       <sheetName val="2016-10-03-5"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2016-01-04-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-40.466640802909239</v>
+          <cell r="I89">
+            <v>-9.3603952065196285</v>
+          </cell>
+          <cell r="M89">
+            <v>-16.985860672015232</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-90.003198143220644</v>
+          <cell r="H92">
+            <v>-5.9482533029348783</v>
+          </cell>
+          <cell r="L92">
+            <v>-26.905048251079528</v>
           </cell>
         </row>
       </sheetData>
@@ -1978,42 +2273,48 @@
     <sheetNames>
       <sheetName val="charts"/>
       <sheetName val="analysis"/>
-      <sheetName val="2017-03-06-4"/>
+      <sheetName val="2016-02-01-5"/>
+      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2016-09-05-4"/>
+      <sheetName val="2016-07-04-4"/>
+      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2016-03-07-4"/>
+      <sheetName val="2015-11-02-5"/>
       <sheetName val="2016-05-02-5"/>
+      <sheetName val="2017-06-05-4"/>
+      <sheetName val="2017-08-07-4"/>
+      <sheetName val="2017-10-02-5"/>
+      <sheetName val="2016-04-04-4"/>
+      <sheetName val="2016-11-07-4"/>
+      <sheetName val="2017-07-03-5"/>
+      <sheetName val="2016-08-01-5"/>
+      <sheetName val="2017-09-04-4"/>
       <sheetName val="2017-04-03-4"/>
-      <sheetName val="2017-07-03-5"/>
-      <sheetName val="2017-06-05-4"/>
-      <sheetName val="2017-05-01-5"/>
+      <sheetName val="2015-12-07-4"/>
+      <sheetName val="2016-01-04-4"/>
+      <sheetName val="2016-10-03-5"/>
       <sheetName val="2016-12-05-5"/>
-      <sheetName val="2016-04-04-4"/>
-      <sheetName val="2016-01-04-4"/>
-      <sheetName val="2016-09-05-4"/>
-      <sheetName val="2017-09-04-4"/>
-      <sheetName val="2016-03-07-4"/>
-      <sheetName val="2015-12-07-4"/>
-      <sheetName val="2016-11-07-4"/>
       <sheetName val="2016-06-06-4"/>
       <sheetName val="2017-02-06-4"/>
-      <sheetName val="2017-10-02-5"/>
-      <sheetName val="2015-11-02-5"/>
-      <sheetName val="2016-10-03-5"/>
-      <sheetName val="2017-08-07-4"/>
-      <sheetName val="2016-08-01-5"/>
-      <sheetName val="2016-02-01-5"/>
-      <sheetName val="2016-07-04-4"/>
-      <sheetName val="2017-01-09-4"/>
+      <sheetName val="2017-03-06-4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="89">
-          <cell r="D89">
-            <v>-39.939328699115599</v>
+          <cell r="I89">
+            <v>-11.03885961703854</v>
+          </cell>
+          <cell r="M89">
+            <v>-15.006777064057978</v>
           </cell>
         </row>
         <row r="92">
-          <cell r="G92">
-            <v>-94.403406283333354</v>
+          <cell r="H92">
+            <v>-14.115539924792179</v>
+          </cell>
+          <cell r="L92">
+            <v>-17.084212574267767</v>
           </cell>
         </row>
       </sheetData>
@@ -2309,10 +2610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,155 +2621,252 @@
     <col min="2" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <f>[1]analysis!G92/100</f>
+        <f>[1]analysis!H92/100</f>
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>[1]analysis!D89/100</f>
+        <f>[1]analysis!I89/100</f>
         <v>0</v>
       </c>
+      <c r="D2" s="2">
+        <f>[1]analysis!L92/100</f>
+        <v>-0.12323057161976494</v>
+      </c>
+      <c r="E2" s="2">
+        <f>[1]analysis!M89/100</f>
+        <v>-9.181563099207686E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
       <c r="B3" s="2">
-        <f>[2]analysis!G92/100</f>
-        <v>-5.224813186635114E-2</v>
+        <f>[2]analysis!H92/100</f>
+        <v>-2.7971027175238614E-2</v>
       </c>
       <c r="C3" s="2">
-        <f>[2]analysis!D89/100</f>
-        <v>-5.6799354798089723E-2</v>
+        <f>[2]analysis!I89/100</f>
+        <v>-3.7178053505118186E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <f>[2]analysis!L92/100</f>
+        <v>-0.23164089300678684</v>
+      </c>
+      <c r="E3" s="2">
+        <f>[2]analysis!M89/100</f>
+        <v>-0.11149714837440589</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.2</v>
       </c>
       <c r="B4" s="2">
-        <f>[3]analysis!G92/100</f>
-        <v>-0.2608652036338539</v>
+        <f>[3]analysis!H92/100</f>
+        <v>5.3382817938382983E-3</v>
       </c>
       <c r="C4" s="2">
-        <f>[3]analysis!D89/100</f>
-        <v>-0.1310855075380663</v>
+        <f>[3]analysis!I89/100</f>
+        <v>-7.9639926728015328E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <f>[3]analysis!L92/100</f>
+        <v>-0.30233649734013579</v>
+      </c>
+      <c r="E4" s="2">
+        <f>[3]analysis!M89/100</f>
+        <v>-0.12457175817247712</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.3</v>
       </c>
       <c r="B5" s="2">
-        <f>[4]analysis!G92/100</f>
-        <v>-0.42117416749225373</v>
+        <f>[4]analysis!H92/100</f>
+        <v>1.6230886980694286E-2</v>
       </c>
       <c r="C5" s="2">
-        <f>[4]analysis!D89/100</f>
-        <v>-0.19854805008087886</v>
+        <f>[4]analysis!I89/100</f>
+        <v>-1.3086940552413839E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <f>[4]analysis!L92/100</f>
+        <v>-0.32328567629518573</v>
+      </c>
+      <c r="E5" s="2">
+        <f>[4]analysis!M89/100</f>
+        <v>-0.11515051463516163</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.4</v>
       </c>
       <c r="B6" s="2">
-        <f>[5]analysis!G92/100</f>
-        <v>-0.66636390050646099</v>
+        <f>[5]analysis!H92/100</f>
+        <v>-6.3418440785472374E-2</v>
       </c>
       <c r="C6" s="2">
-        <f>[5]analysis!D89/100</f>
-        <v>-0.2364802448653196</v>
+        <f>[5]analysis!I89/100</f>
+        <v>-2.2227778622953397E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <f>[5]analysis!L92/100</f>
+        <v>-0.21298388953801081</v>
+      </c>
+      <c r="E6" s="2">
+        <f>[5]analysis!M89/100</f>
+        <v>-0.12231013154534005</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.5</v>
       </c>
       <c r="B7" s="2">
-        <f>[6]analysis!G92/100</f>
-        <v>-0.67958437524874538</v>
+        <f>[6]analysis!H92/100</f>
+        <v>-1.4540055900507096E-2</v>
       </c>
       <c r="C7" s="2">
-        <f>[6]analysis!D89/100</f>
-        <v>-0.29684368483689794</v>
+        <f>[6]analysis!I89/100</f>
+        <v>-5.8178070445915601E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <f>[6]analysis!L92/100</f>
+        <v>-0.10802485383342604</v>
+      </c>
+      <c r="E7" s="2">
+        <f>[6]analysis!M89/100</f>
+        <v>-0.15100636878708529</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.6</v>
       </c>
       <c r="B8" s="2">
-        <f>[7]analysis!G92/100</f>
-        <v>-0.76693053914773313</v>
+        <f>[7]analysis!H92/100</f>
+        <v>-4.1596161053225299E-2</v>
       </c>
       <c r="C8" s="2">
-        <f>[7]analysis!D89/100</f>
-        <v>-0.3675586126986351</v>
+        <f>[7]analysis!I89/100</f>
+        <v>-7.8348751953718293E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <f>[7]analysis!L92/100</f>
+        <v>-0.1449782781520764</v>
+      </c>
+      <c r="E8" s="2">
+        <f>[7]analysis!M89/100</f>
+        <v>-0.15075297494221235</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.7</v>
       </c>
       <c r="B9" s="2">
-        <f>[8]analysis!G92/100</f>
-        <v>-0.90003198143220642</v>
+        <f>[8]analysis!H92/100</f>
+        <v>-5.9482533029348784E-2</v>
       </c>
       <c r="C9" s="2">
-        <f>[8]analysis!D89/100</f>
-        <v>-0.40466640802909237</v>
+        <f>[8]analysis!I89/100</f>
+        <v>-9.3603952065196283E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <f>[8]analysis!L92/100</f>
+        <v>-0.26905048251079527</v>
+      </c>
+      <c r="E9" s="2">
+        <f>[8]analysis!M89/100</f>
+        <v>-0.16985860672015232</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.8</v>
       </c>
       <c r="B10" s="2">
-        <f>[9]analysis!G92/100</f>
-        <v>-0.94403406283333358</v>
+        <f>[9]analysis!H92/100</f>
+        <v>-0.14115539924792178</v>
       </c>
       <c r="C10" s="2">
-        <f>[9]analysis!D89/100</f>
-        <v>-0.399393286991156</v>
+        <f>[9]analysis!I89/100</f>
+        <v>-0.11038859617038539</v>
+      </c>
+      <c r="D10" s="2">
+        <f>[9]analysis!L92/100</f>
+        <v>-0.17084212574267765</v>
+      </c>
+      <c r="E10" s="2">
+        <f>[9]analysis!M89/100</f>
+        <v>-0.15006777064057977</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.9</v>
       </c>
       <c r="B11" s="2">
-        <f>[10]analysis!G92/100</f>
-        <v>-0.96496810778391373</v>
+        <f>[10]analysis!H92/100</f>
+        <v>-0.15566662571041948</v>
       </c>
       <c r="C11" s="2">
-        <f>[10]analysis!D89/100</f>
-        <v>-0.42878842634149705</v>
+        <f>[10]analysis!I89/100</f>
+        <v>-0.13492473240673331</v>
+      </c>
+      <c r="D11" s="2">
+        <f>[10]analysis!L92/100</f>
+        <v>-0.16615310187323939</v>
+      </c>
+      <c r="E11" s="2">
+        <f>[10]analysis!M89/100</f>
+        <v>-0.14708943076262754</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" s="2">
-        <f>[11]analysis!G92/100</f>
-        <v>-0.99641276837750237</v>
+        <f>[11]analysis!H92/100</f>
+        <v>-7.7783515544197671E-2</v>
       </c>
       <c r="C12" s="2">
-        <f>[11]analysis!D89/100</f>
-        <v>-0.77475110588747431</v>
+        <f>[11]analysis!I89/100</f>
+        <v>-0.11726771819964622</v>
+      </c>
+      <c r="D12" s="2">
+        <f>[11]analysis!L92/100</f>
+        <v>-0.39300916062583441</v>
+      </c>
+      <c r="E12" s="2">
+        <f>[11]analysis!M89/100</f>
+        <v>-0.24416150652844293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add results for different target preference rates
</commit_message>
<xml_diff>
--- a/results/conf_progression.xlsx
+++ b/results/conf_progression.xlsx
@@ -593,11 +593,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="173086432"/>
-        <c:axId val="173085344"/>
+        <c:axId val="-547732832"/>
+        <c:axId val="-547732288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173086432"/>
+        <c:axId val="-547732832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +688,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173085344"/>
+        <c:crossAx val="-547732288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -696,7 +696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173085344"/>
+        <c:axId val="-547732288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -736,7 +736,7 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>relative difference for ESD to C</a:t>
+                  <a:t>relative difference for ESL to CL</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -768,7 +768,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -796,9 +796,9 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173086432"/>
+        <c:crossAx val="-547732832"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -826,10 +826,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="LM Roman 9" panose="00000500000000000000" pitchFamily="50" charset="0"/>
               <a:ea typeface="+mn-ea"/>
@@ -2612,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add data, results and code as used in paper
</commit_message>
<xml_diff>
--- a/results/conf_progression.xlsx
+++ b/results/conf_progression.xlsx
@@ -593,11 +593,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-547732832"/>
-        <c:axId val="-547732288"/>
+        <c:axId val="-1553009680"/>
+        <c:axId val="-1553008592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-547732832"/>
+        <c:axId val="-1553009680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +688,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-547732288"/>
+        <c:crossAx val="-1553008592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -696,7 +696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-547732288"/>
+        <c:axId val="-1553008592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -736,7 +736,7 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>relative difference for ESL to CL</a:t>
+                  <a:t>relative difference for F-ESL to F-CL</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -796,7 +796,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-547732832"/>
+        <c:crossAx val="-1553009680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2609,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>